<commit_message>
Prepared dataframes of historical and 2018 startups.
</commit_message>
<xml_diff>
--- a/swisscom/data/WinnerStartups2017.xlsx
+++ b/swisscom/data/WinnerStartups2017.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="4260" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
+    <workbookView xWindow="640" yWindow="1180" windowWidth="28160" windowHeight="16820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -861,13 +861,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -1149,10 +1150,13 @@
   <dimension ref="A1:C201"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.6640625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
@@ -1166,223 +1170,223 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+      <c r="A2" s="4">
         <v>1</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="4" t="s">
+      <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2" t="s">
+      <c r="A3" s="4"/>
+      <c r="B3" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="4"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5">
+      <c r="A4" s="4">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
+      <c r="A5" s="4"/>
       <c r="B5" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C5" s="4"/>
+      <c r="C5" s="3"/>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5">
+      <c r="A6" s="4">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="3" t="s">
         <v>8</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
+      <c r="A7" s="4"/>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="4"/>
+      <c r="C7" s="3"/>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5">
+      <c r="A8" s="4">
         <v>4</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="3" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
+      <c r="A9" s="4"/>
       <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C9" s="4"/>
+      <c r="C9" s="3"/>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="5">
+      <c r="A10" s="4">
         <v>5</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C10" s="4" t="s">
+      <c r="C10" s="3" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="5"/>
+      <c r="A11" s="4"/>
       <c r="B11" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C11" s="4"/>
+      <c r="C11" s="3"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5">
+      <c r="A12" s="4">
         <v>6</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C12" s="4" t="s">
+      <c r="C12" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A13" s="5"/>
+      <c r="A13" s="4"/>
       <c r="B13" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C13" s="4"/>
+      <c r="C13" s="3"/>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A14" s="5">
+      <c r="A14" s="4">
         <v>7</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C14" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A15" s="5"/>
+      <c r="A15" s="4"/>
       <c r="B15" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="4"/>
+      <c r="C15" s="3"/>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A16" s="5">
+      <c r="A16" s="4">
         <v>8</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="C16" s="4" t="s">
+      <c r="C16" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A17" s="5"/>
+      <c r="A17" s="4"/>
       <c r="B17" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C17" s="4"/>
+      <c r="C17" s="3"/>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A18" s="5">
+      <c r="A18" s="4">
         <v>9</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="4" t="s">
+      <c r="C18" s="3" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A19" s="5"/>
+      <c r="A19" s="4"/>
       <c r="B19" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="4"/>
+      <c r="C19" s="3"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A20" s="5">
+      <c r="A20" s="4">
         <v>10</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A21" s="5"/>
+      <c r="A21" s="4"/>
       <c r="B21" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C21" s="4"/>
+      <c r="C21" s="3"/>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A22" s="5">
+      <c r="A22" s="4">
         <v>11</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A23" s="5"/>
+      <c r="A23" s="4"/>
       <c r="B23" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="4"/>
+      <c r="C23" s="3"/>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A24" s="5">
+      <c r="A24" s="4">
         <v>12</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C24" s="3" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A25" s="5"/>
+      <c r="A25" s="4"/>
       <c r="B25" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C25" s="4"/>
+      <c r="C25" s="3"/>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A26" s="5">
+      <c r="A26" s="4">
         <v>13</v>
       </c>
       <c r="B26" s="1" t="s">
@@ -1393,7 +1397,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A27" s="5"/>
+      <c r="A27" s="4"/>
       <c r="B27" s="2" t="s">
         <v>34</v>
       </c>
@@ -1402,455 +1406,455 @@
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A28" s="5">
+      <c r="A28" s="4">
         <v>14</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C28" s="3" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A29" s="5"/>
+      <c r="A29" s="4"/>
       <c r="B29" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C29" s="4"/>
+      <c r="C29" s="3"/>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A30" s="5">
+      <c r="A30" s="4">
         <v>15</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>40</v>
       </c>
-      <c r="C30" s="4" t="s">
+      <c r="C30" s="3" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A31" s="5"/>
+      <c r="A31" s="4"/>
       <c r="B31" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C31" s="4"/>
+      <c r="C31" s="3"/>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A32" s="5">
+      <c r="A32" s="4">
         <v>16</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>42</v>
       </c>
-      <c r="C32" s="4" t="s">
+      <c r="C32" s="3" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A33" s="5"/>
+      <c r="A33" s="4"/>
       <c r="B33" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C33" s="4"/>
+      <c r="C33" s="3"/>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A34" s="5">
+      <c r="A34" s="4">
         <v>17</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C34" s="4" t="s">
+      <c r="C34" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A35" s="5"/>
+      <c r="A35" s="4"/>
       <c r="B35" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C35" s="4"/>
+      <c r="C35" s="3"/>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A36" s="5">
+      <c r="A36" s="4">
         <v>18</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C36" s="4" t="s">
+      <c r="C36" s="3" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A37" s="5"/>
+      <c r="A37" s="4"/>
       <c r="B37" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C37" s="4"/>
+      <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A38" s="5">
+      <c r="A38" s="4">
         <v>19</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="3" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A39" s="5"/>
+      <c r="A39" s="4"/>
       <c r="B39" s="2" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="4"/>
+      <c r="C39" s="3"/>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" s="5">
+      <c r="A40" s="4">
         <v>20</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C40" s="4" t="s">
+      <c r="C40" s="3" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" s="5"/>
+      <c r="A41" s="4"/>
       <c r="B41" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C41" s="4"/>
+      <c r="C41" s="3"/>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" s="5">
+      <c r="A42" s="4">
         <v>21</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>57</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C42" s="3" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A43" s="5"/>
+      <c r="A43" s="4"/>
       <c r="B43" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="C43" s="4"/>
+      <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A44" s="5">
+      <c r="A44" s="4">
         <v>22</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>60</v>
       </c>
-      <c r="C44" s="4" t="s">
+      <c r="C44" s="3" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A45" s="5"/>
+      <c r="A45" s="4"/>
       <c r="B45" s="2" t="s">
         <v>61</v>
       </c>
-      <c r="C45" s="4"/>
+      <c r="C45" s="3"/>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A46" s="5">
+      <c r="A46" s="4">
         <v>23</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="C46" s="4" t="s">
+      <c r="C46" s="3" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A47" s="5"/>
+      <c r="A47" s="4"/>
       <c r="B47" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C47" s="4"/>
+      <c r="C47" s="3"/>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A48" s="5">
+      <c r="A48" s="4">
         <v>24</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="C48" s="4" t="s">
+      <c r="C48" s="3" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A49" s="5"/>
+      <c r="A49" s="4"/>
       <c r="B49" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C49" s="4"/>
+      <c r="C49" s="3"/>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A50" s="5">
+      <c r="A50" s="4">
         <v>25</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>67</v>
       </c>
-      <c r="C50" s="4" t="s">
+      <c r="C50" s="3" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A51" s="5"/>
+      <c r="A51" s="4"/>
       <c r="B51" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C51" s="4"/>
+      <c r="C51" s="3"/>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A52" s="5">
+      <c r="A52" s="4">
         <v>26</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="C52" s="4" t="s">
+      <c r="C52" s="3" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A53" s="5"/>
+      <c r="A53" s="4"/>
       <c r="B53" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="C53" s="4"/>
+      <c r="C53" s="3"/>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A54" s="5">
+      <c r="A54" s="4">
         <v>27</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="4" t="s">
+      <c r="C54" s="3" t="s">
         <v>73</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A55" s="5"/>
+      <c r="A55" s="4"/>
       <c r="B55" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C55" s="4"/>
+      <c r="C55" s="3"/>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A56" s="5">
+      <c r="A56" s="4">
         <v>28</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C56" s="4"/>
+      <c r="C56" s="3"/>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A57" s="5"/>
+      <c r="A57" s="4"/>
       <c r="B57" s="2" t="s">
         <v>75</v>
       </c>
-      <c r="C57" s="4"/>
+      <c r="C57" s="3"/>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A58" s="5">
+      <c r="A58" s="4">
         <v>29</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="C58" s="4" t="s">
+      <c r="C58" s="3" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A59" s="5"/>
+      <c r="A59" s="4"/>
       <c r="B59" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C59" s="4"/>
+      <c r="C59" s="3"/>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A60" s="5">
+      <c r="A60" s="4">
         <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="C60" s="4" t="s">
+      <c r="C60" s="3" t="s">
         <v>79</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A61" s="5"/>
+      <c r="A61" s="4"/>
       <c r="B61" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C61" s="4"/>
+      <c r="C61" s="3"/>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A62" s="5">
+      <c r="A62" s="4">
         <v>31</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="C62" s="4" t="s">
+      <c r="C62" s="3" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A63" s="5"/>
+      <c r="A63" s="4"/>
       <c r="B63" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C63" s="4"/>
+      <c r="C63" s="3"/>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A64" s="5">
+      <c r="A64" s="4">
         <v>32</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="C64" s="4" t="s">
+      <c r="C64" s="3" t="s">
         <v>84</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A65" s="5"/>
+      <c r="A65" s="4"/>
       <c r="B65" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="4"/>
+      <c r="C65" s="3"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A66" s="5">
+      <c r="A66" s="4">
         <v>33</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>85</v>
       </c>
-      <c r="C66" s="4" t="s">
+      <c r="C66" s="3" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A67" s="5"/>
+      <c r="A67" s="4"/>
       <c r="B67" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C67" s="4"/>
+      <c r="C67" s="3"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A68" s="5">
+      <c r="A68" s="4">
         <v>34</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="C68" s="4" t="s">
+      <c r="C68" s="3" t="s">
         <v>90</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A69" s="5"/>
+      <c r="A69" s="4"/>
       <c r="B69" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="4"/>
+      <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A70" s="5">
+      <c r="A70" s="4">
         <v>35</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C70" s="4" t="s">
+      <c r="C70" s="3" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A71" s="5"/>
+      <c r="A71" s="4"/>
       <c r="B71" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C71" s="4"/>
+      <c r="C71" s="3"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A72" s="5">
+      <c r="A72" s="4">
         <v>36</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>93</v>
       </c>
-      <c r="C72" s="4" t="s">
+      <c r="C72" s="3" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A73" s="5"/>
+      <c r="A73" s="4"/>
       <c r="B73" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C73" s="4"/>
+      <c r="C73" s="3"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A74" s="5">
+      <c r="A74" s="4">
         <v>37</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>96</v>
       </c>
-      <c r="C74" s="4" t="s">
+      <c r="C74" s="3" t="s">
         <v>97</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A75" s="5"/>
+      <c r="A75" s="4"/>
       <c r="B75" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C75" s="4"/>
+      <c r="C75" s="3"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A76" s="5">
+      <c r="A76" s="4">
         <v>38</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>98</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C76" s="3" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A77" s="5"/>
+      <c r="A77" s="4"/>
       <c r="B77" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C77" s="4"/>
+      <c r="C77" s="3"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A78" s="5">
+      <c r="A78" s="4">
         <v>39</v>
       </c>
       <c r="B78" s="1" t="s">
@@ -1861,7 +1865,7 @@
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A79" s="5"/>
+      <c r="A79" s="4"/>
       <c r="B79" s="2" t="s">
         <v>1</v>
       </c>
@@ -1870,1304 +1874,1104 @@
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A80" s="5">
+      <c r="A80" s="4">
         <v>40</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="C80" s="4" t="s">
+      <c r="C80" s="3" t="s">
         <v>105</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A81" s="5"/>
+      <c r="A81" s="4"/>
       <c r="B81" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C81" s="4"/>
+      <c r="C81" s="3"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A82" s="5">
+      <c r="A82" s="4">
         <v>41</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C82" s="3" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A83" s="5"/>
+      <c r="A83" s="4"/>
       <c r="B83" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C83" s="4"/>
+      <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A84" s="5">
+      <c r="A84" s="4">
         <v>42</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>108</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C84" s="3" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A85" s="5"/>
+      <c r="A85" s="4"/>
       <c r="B85" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C85" s="4"/>
+      <c r="C85" s="3"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A86" s="5">
+      <c r="A86" s="4">
         <v>43</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>111</v>
       </c>
-      <c r="C86" s="4" t="s">
+      <c r="C86" s="3" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A87" s="5"/>
+      <c r="A87" s="4"/>
       <c r="B87" s="2" t="s">
         <v>112</v>
       </c>
-      <c r="C87" s="4"/>
+      <c r="C87" s="3"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A88" s="5">
+      <c r="A88" s="4">
         <v>44</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>114</v>
       </c>
-      <c r="C88" s="4" t="s">
+      <c r="C88" s="3" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A89" s="5"/>
+      <c r="A89" s="4"/>
       <c r="B89" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C89" s="4"/>
+      <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A90" s="5">
+      <c r="A90" s="4">
         <v>45</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>117</v>
       </c>
-      <c r="C90" s="4" t="s">
+      <c r="C90" s="3" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A91" s="5"/>
+      <c r="A91" s="4"/>
       <c r="B91" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C91" s="4"/>
+      <c r="C91" s="3"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A92" s="5">
+      <c r="A92" s="4">
         <v>46</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="C92" s="4" t="s">
+      <c r="C92" s="3" t="s">
         <v>121</v>
       </c>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A93" s="5"/>
+      <c r="A93" s="4"/>
       <c r="B93" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C93" s="4"/>
+      <c r="C93" s="3"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A94" s="5">
+      <c r="A94" s="4">
         <v>47</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="C94" s="4" t="s">
+      <c r="C94" s="3" t="s">
         <v>124</v>
       </c>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A95" s="5"/>
+      <c r="A95" s="4"/>
       <c r="B95" s="2" t="s">
         <v>123</v>
       </c>
-      <c r="C95" s="4"/>
+      <c r="C95" s="3"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A96" s="5">
+      <c r="A96" s="4">
         <v>48</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>125</v>
       </c>
-      <c r="C96" s="4" t="s">
+      <c r="C96" s="3" t="s">
         <v>127</v>
       </c>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A97" s="5"/>
+      <c r="A97" s="4"/>
       <c r="B97" s="2" t="s">
         <v>126</v>
       </c>
-      <c r="C97" s="4"/>
+      <c r="C97" s="3"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A98" s="5">
+      <c r="A98" s="4">
         <v>49</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C98" s="4" t="s">
+      <c r="C98" s="3" t="s">
         <v>129</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A99" s="5"/>
+      <c r="A99" s="4"/>
       <c r="B99" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C99" s="4"/>
+      <c r="C99" s="3"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A100" s="5">
+      <c r="A100" s="4">
         <v>50</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>130</v>
       </c>
-      <c r="C100" s="4" t="s">
+      <c r="C100" s="3" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A101" s="5"/>
+      <c r="A101" s="4"/>
       <c r="B101" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="C101" s="4"/>
+      <c r="C101" s="3"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A102" s="5">
+      <c r="A102" s="4">
         <v>51</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C102" s="4" t="s">
+      <c r="C102" s="3" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A103" s="5"/>
+      <c r="A103" s="4"/>
       <c r="B103" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="C103" s="4"/>
+      <c r="C103" s="3"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A104" s="5">
+      <c r="A104" s="4">
         <v>52</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="C104" s="4" t="s">
+      <c r="C104" s="3" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A105" s="5"/>
+      <c r="A105" s="4"/>
       <c r="B105" s="2" t="s">
         <v>137</v>
       </c>
-      <c r="C105" s="4"/>
+      <c r="C105" s="3"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A106" s="5">
+      <c r="A106" s="4">
         <v>53</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>139</v>
       </c>
-      <c r="C106" s="4" t="s">
+      <c r="C106" s="3" t="s">
         <v>140</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A107" s="5"/>
+      <c r="A107" s="4"/>
       <c r="B107" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C107" s="4"/>
+      <c r="C107" s="3"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A108" s="5">
+      <c r="A108" s="4">
         <v>54</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>141</v>
       </c>
-      <c r="C108" s="4" t="s">
+      <c r="C108" s="3" t="s">
         <v>142</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A109" s="5"/>
+      <c r="A109" s="4"/>
       <c r="B109" s="2" t="s">
         <v>55</v>
       </c>
-      <c r="C109" s="4"/>
+      <c r="C109" s="3"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A110" s="5">
+      <c r="A110" s="4">
         <v>55</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="C110" s="4" t="s">
+      <c r="C110" s="3" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A111" s="5"/>
+      <c r="A111" s="4"/>
       <c r="B111" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="C111" s="4"/>
+      <c r="C111" s="3"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A112" s="5">
+      <c r="A112" s="4">
         <v>56</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="C112" s="4" t="s">
+      <c r="C112" s="3" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A113" s="5"/>
+      <c r="A113" s="4"/>
       <c r="B113" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="C113" s="4"/>
+      <c r="C113" s="3"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A114" s="5">
+      <c r="A114" s="4">
         <v>57</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="C114" s="4" t="s">
+      <c r="C114" s="3" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A115" s="5"/>
+      <c r="A115" s="4"/>
       <c r="B115" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C115" s="4"/>
+      <c r="C115" s="3"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A116" s="5">
+      <c r="A116" s="4">
         <v>58</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>151</v>
       </c>
-      <c r="C116" s="4" t="s">
+      <c r="C116" s="3" t="s">
         <v>152</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A117" s="5"/>
+      <c r="A117" s="4"/>
       <c r="B117" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C117" s="4"/>
+      <c r="C117" s="3"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A118" s="5">
+      <c r="A118" s="4">
         <v>59</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>153</v>
       </c>
-      <c r="C118" s="4" t="s">
+      <c r="C118" s="3" t="s">
         <v>155</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A119" s="5"/>
+      <c r="A119" s="4"/>
       <c r="B119" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C119" s="4"/>
+      <c r="C119" s="3"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A120" s="5">
+      <c r="A120" s="4">
         <v>60</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>156</v>
       </c>
-      <c r="C120" s="4" t="s">
+      <c r="C120" s="3" t="s">
         <v>158</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A121" s="5"/>
+      <c r="A121" s="4"/>
       <c r="B121" s="2" t="s">
         <v>157</v>
       </c>
-      <c r="C121" s="4"/>
+      <c r="C121" s="3"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A122" s="5">
+      <c r="A122" s="4">
         <v>61</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="C122" s="4" t="s">
+      <c r="C122" s="3" t="s">
         <v>160</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A123" s="5"/>
+      <c r="A123" s="4"/>
       <c r="B123" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C123" s="4"/>
+      <c r="C123" s="3"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A124" s="5">
+      <c r="A124" s="4">
         <v>62</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="C124" s="4" t="s">
+      <c r="C124" s="3" t="s">
         <v>163</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A125" s="5"/>
+      <c r="A125" s="4"/>
       <c r="B125" s="2" t="s">
         <v>162</v>
       </c>
-      <c r="C125" s="4"/>
+      <c r="C125" s="3"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A126" s="5">
+      <c r="A126" s="4">
         <v>63</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>164</v>
       </c>
-      <c r="C126" s="4" t="s">
+      <c r="C126" s="3" t="s">
         <v>166</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A127" s="5"/>
+      <c r="A127" s="4"/>
       <c r="B127" s="2" t="s">
         <v>165</v>
       </c>
-      <c r="C127" s="4"/>
+      <c r="C127" s="3"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A128" s="5">
+      <c r="A128" s="4">
         <v>64</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>167</v>
       </c>
-      <c r="C128" s="4" t="s">
+      <c r="C128" s="3" t="s">
         <v>169</v>
       </c>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A129" s="5"/>
+      <c r="A129" s="4"/>
       <c r="B129" s="2" t="s">
         <v>168</v>
       </c>
-      <c r="C129" s="4"/>
+      <c r="C129" s="3"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A130" s="5">
+      <c r="A130" s="4">
         <v>65</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C130" s="4" t="s">
+      <c r="C130" s="3" t="s">
         <v>172</v>
       </c>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A131" s="5"/>
+      <c r="A131" s="4"/>
       <c r="B131" s="2" t="s">
         <v>171</v>
       </c>
-      <c r="C131" s="4"/>
+      <c r="C131" s="3"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A132" s="5">
+      <c r="A132" s="4">
         <v>66</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="C132" s="4" t="s">
+      <c r="C132" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A133" s="5"/>
+      <c r="A133" s="4"/>
       <c r="B133" s="2" t="s">
         <v>154</v>
       </c>
-      <c r="C133" s="4"/>
+      <c r="C133" s="3"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A134" s="5">
+      <c r="A134" s="4">
         <v>67</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>175</v>
       </c>
-      <c r="C134" s="4" t="s">
+      <c r="C134" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A135" s="5"/>
+      <c r="A135" s="4"/>
       <c r="B135" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C135" s="4"/>
+      <c r="C135" s="3"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A136" s="5">
+      <c r="A136" s="4">
         <v>68</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>177</v>
       </c>
-      <c r="C136" s="4" t="s">
+      <c r="C136" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A137" s="5"/>
+      <c r="A137" s="4"/>
       <c r="B137" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C137" s="4"/>
+      <c r="C137" s="3"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A138" s="5">
+      <c r="A138" s="4">
         <v>69</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>179</v>
       </c>
-      <c r="C138" s="4" t="s">
+      <c r="C138" s="3" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A139" s="5"/>
+      <c r="A139" s="4"/>
       <c r="B139" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C139" s="4"/>
+      <c r="C139" s="3"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A140" s="5">
+      <c r="A140" s="4">
         <v>70</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>181</v>
       </c>
-      <c r="C140" s="4" t="s">
+      <c r="C140" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A141" s="5"/>
+      <c r="A141" s="4"/>
       <c r="B141" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C141" s="4"/>
+      <c r="C141" s="3"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A142" s="5">
+      <c r="A142" s="4">
         <v>71</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>183</v>
       </c>
-      <c r="C142" s="4" t="s">
+      <c r="C142" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A143" s="5"/>
+      <c r="A143" s="4"/>
       <c r="B143" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C143" s="4"/>
+      <c r="C143" s="3"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A144" s="5">
+      <c r="A144" s="4">
         <v>72</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="C144" s="4" t="s">
+      <c r="C144" s="3" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="145" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A145" s="5"/>
+      <c r="A145" s="4"/>
       <c r="B145" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="C145" s="4"/>
+      <c r="C145" s="3"/>
     </row>
     <row r="146" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A146" s="5">
+      <c r="A146" s="4">
         <v>73</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>187</v>
       </c>
-      <c r="C146" s="4" t="s">
+      <c r="C146" s="3" t="s">
         <v>189</v>
       </c>
     </row>
     <row r="147" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A147" s="5"/>
+      <c r="A147" s="4"/>
       <c r="B147" s="2" t="s">
         <v>188</v>
       </c>
-      <c r="C147" s="4"/>
+      <c r="C147" s="3"/>
     </row>
     <row r="148" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A148" s="5">
+      <c r="A148" s="4">
         <v>74</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>190</v>
       </c>
-      <c r="C148" s="4" t="s">
+      <c r="C148" s="3" t="s">
         <v>192</v>
       </c>
     </row>
     <row r="149" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A149" s="5"/>
+      <c r="A149" s="4"/>
       <c r="B149" s="2" t="s">
         <v>191</v>
       </c>
-      <c r="C149" s="4"/>
+      <c r="C149" s="3"/>
     </row>
     <row r="150" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A150" s="5">
+      <c r="A150" s="4">
         <v>75</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>193</v>
       </c>
-      <c r="C150" s="4" t="s">
+      <c r="C150" s="3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="151" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A151" s="5"/>
+      <c r="A151" s="4"/>
       <c r="B151" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C151" s="4"/>
+      <c r="C151" s="3"/>
     </row>
     <row r="152" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A152" s="5">
+      <c r="A152" s="4">
         <v>76</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>195</v>
       </c>
-      <c r="C152" s="4" t="s">
+      <c r="C152" s="3" t="s">
         <v>196</v>
       </c>
     </row>
     <row r="153" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A153" s="5"/>
+      <c r="A153" s="4"/>
       <c r="B153" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C153" s="4"/>
+      <c r="C153" s="3"/>
     </row>
     <row r="154" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A154" s="5">
+      <c r="A154" s="4">
         <v>77</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>197</v>
       </c>
-      <c r="C154" s="4" t="s">
+      <c r="C154" s="3" t="s">
         <v>199</v>
       </c>
     </row>
     <row r="155" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A155" s="5"/>
+      <c r="A155" s="4"/>
       <c r="B155" s="2" t="s">
         <v>198</v>
       </c>
-      <c r="C155" s="4"/>
+      <c r="C155" s="3"/>
     </row>
     <row r="156" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A156" s="5">
+      <c r="A156" s="4">
         <v>78</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>200</v>
       </c>
-      <c r="C156" s="4" t="s">
+      <c r="C156" s="3" t="s">
         <v>202</v>
       </c>
     </row>
     <row r="157" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A157" s="5"/>
+      <c r="A157" s="4"/>
       <c r="B157" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C157" s="4"/>
+      <c r="C157" s="3"/>
     </row>
     <row r="158" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A158" s="5">
+      <c r="A158" s="4">
         <v>79</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>203</v>
       </c>
-      <c r="C158" s="4" t="s">
+      <c r="C158" s="3" t="s">
         <v>205</v>
       </c>
     </row>
     <row r="159" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A159" s="5"/>
+      <c r="A159" s="4"/>
       <c r="B159" s="2" t="s">
         <v>204</v>
       </c>
-      <c r="C159" s="4"/>
+      <c r="C159" s="3"/>
     </row>
     <row r="160" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A160" s="5">
+      <c r="A160" s="4">
         <v>80</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>206</v>
       </c>
-      <c r="C160" s="4" t="s">
+      <c r="C160" s="3" t="s">
         <v>207</v>
       </c>
     </row>
     <row r="161" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A161" s="5"/>
+      <c r="A161" s="4"/>
       <c r="B161" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C161" s="4"/>
+      <c r="C161" s="3"/>
     </row>
     <row r="162" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A162" s="5">
+      <c r="A162" s="4">
         <v>81</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>208</v>
       </c>
-      <c r="C162" s="4" t="s">
+      <c r="C162" s="3" t="s">
         <v>209</v>
       </c>
     </row>
     <row r="163" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A163" s="5"/>
+      <c r="A163" s="4"/>
       <c r="B163" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C163" s="4"/>
+      <c r="C163" s="3"/>
     </row>
     <row r="164" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A164" s="5">
+      <c r="A164" s="4">
         <v>82</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>210</v>
       </c>
-      <c r="C164" s="4" t="s">
+      <c r="C164" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="165" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A165" s="5"/>
+      <c r="A165" s="4"/>
       <c r="B165" s="2" t="s">
         <v>211</v>
       </c>
-      <c r="C165" s="4"/>
+      <c r="C165" s="3"/>
     </row>
     <row r="166" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A166" s="5">
+      <c r="A166" s="4">
         <v>83</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>213</v>
       </c>
-      <c r="C166" s="4" t="s">
+      <c r="C166" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="167" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A167" s="5"/>
+      <c r="A167" s="4"/>
       <c r="B167" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C167" s="4"/>
+      <c r="C167" s="3"/>
     </row>
     <row r="168" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A168" s="5">
+      <c r="A168" s="4">
         <v>84</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="C168" s="4" t="s">
+      <c r="C168" s="3" t="s">
         <v>216</v>
       </c>
     </row>
     <row r="169" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A169" s="5"/>
+      <c r="A169" s="4"/>
       <c r="B169" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C169" s="4"/>
+      <c r="C169" s="3"/>
     </row>
     <row r="170" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A170" s="5">
+      <c r="A170" s="4">
         <v>85</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>217</v>
       </c>
-      <c r="C170" s="4" t="s">
+      <c r="C170" s="3" t="s">
         <v>218</v>
       </c>
     </row>
     <row r="171" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A171" s="5"/>
+      <c r="A171" s="4"/>
       <c r="B171" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C171" s="4"/>
+      <c r="C171" s="3"/>
     </row>
     <row r="172" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A172" s="5">
+      <c r="A172" s="4">
         <v>86</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>219</v>
       </c>
-      <c r="C172" s="4" t="s">
+      <c r="C172" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="173" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A173" s="5"/>
+      <c r="A173" s="4"/>
       <c r="B173" s="2" t="s">
         <v>115</v>
       </c>
-      <c r="C173" s="4"/>
+      <c r="C173" s="3"/>
     </row>
     <row r="174" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A174" s="5">
+      <c r="A174" s="4">
         <v>87</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>221</v>
       </c>
-      <c r="C174" s="4" t="s">
+      <c r="C174" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="175" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A175" s="5"/>
+      <c r="A175" s="4"/>
       <c r="B175" s="2" t="s">
         <v>222</v>
       </c>
-      <c r="C175" s="4"/>
+      <c r="C175" s="3"/>
     </row>
     <row r="176" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A176" s="5">
+      <c r="A176" s="4">
         <v>88</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>224</v>
       </c>
-      <c r="C176" s="4" t="s">
+      <c r="C176" s="3" t="s">
         <v>225</v>
       </c>
     </row>
     <row r="177" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A177" s="5"/>
+      <c r="A177" s="4"/>
       <c r="B177" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="C177" s="4"/>
+      <c r="C177" s="3"/>
     </row>
     <row r="178" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A178" s="5">
+      <c r="A178" s="4">
         <v>89</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>226</v>
       </c>
-      <c r="C178" s="4" t="s">
+      <c r="C178" s="3" t="s">
         <v>228</v>
       </c>
     </row>
     <row r="179" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A179" s="5"/>
+      <c r="A179" s="4"/>
       <c r="B179" s="2" t="s">
         <v>227</v>
       </c>
-      <c r="C179" s="4"/>
+      <c r="C179" s="3"/>
     </row>
     <row r="180" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A180" s="5">
+      <c r="A180" s="4">
         <v>90</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>229</v>
       </c>
-      <c r="C180" s="4" t="s">
+      <c r="C180" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="181" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A181" s="5"/>
+      <c r="A181" s="4"/>
       <c r="B181" s="2" t="s">
         <v>230</v>
       </c>
-      <c r="C181" s="4"/>
+      <c r="C181" s="3"/>
     </row>
     <row r="182" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A182" s="5">
+      <c r="A182" s="4">
         <v>91</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>232</v>
       </c>
-      <c r="C182" s="4" t="s">
+      <c r="C182" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="183" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A183" s="5"/>
+      <c r="A183" s="4"/>
       <c r="B183" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="C183" s="4"/>
+      <c r="C183" s="3"/>
     </row>
     <row r="184" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A184" s="5">
+      <c r="A184" s="4">
         <v>92</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>234</v>
       </c>
-      <c r="C184" s="4" t="s">
+      <c r="C184" s="3" t="s">
         <v>235</v>
       </c>
     </row>
     <row r="185" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A185" s="5"/>
+      <c r="A185" s="4"/>
       <c r="B185" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C185" s="4"/>
+      <c r="C185" s="3"/>
     </row>
     <row r="186" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A186" s="5">
+      <c r="A186" s="4">
         <v>93</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>236</v>
       </c>
-      <c r="C186" s="4" t="s">
+      <c r="C186" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="187" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A187" s="5"/>
+      <c r="A187" s="4"/>
       <c r="B187" s="2" t="s">
         <v>237</v>
       </c>
-      <c r="C187" s="4"/>
+      <c r="C187" s="3"/>
     </row>
     <row r="188" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A188" s="5">
+      <c r="A188" s="4">
         <v>94</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>239</v>
       </c>
-      <c r="C188" s="4" t="s">
+      <c r="C188" s="3" t="s">
         <v>240</v>
       </c>
     </row>
     <row r="189" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A189" s="5"/>
+      <c r="A189" s="4"/>
       <c r="B189" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C189" s="4"/>
+      <c r="C189" s="3"/>
     </row>
     <row r="190" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A190" s="5">
+      <c r="A190" s="4">
         <v>95</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>241</v>
       </c>
-      <c r="C190" s="4" t="s">
+      <c r="C190" s="3" t="s">
         <v>242</v>
       </c>
     </row>
     <row r="191" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A191" s="5"/>
+      <c r="A191" s="4"/>
       <c r="B191" s="2" t="s">
         <v>118</v>
       </c>
-      <c r="C191" s="4"/>
+      <c r="C191" s="3"/>
     </row>
     <row r="192" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A192" s="5">
+      <c r="A192" s="4">
         <v>96</v>
       </c>
       <c r="B192" s="1" t="s">
         <v>243</v>
       </c>
-      <c r="C192" s="4" t="s">
+      <c r="C192" s="3" t="s">
         <v>244</v>
       </c>
     </row>
     <row r="193" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A193" s="5"/>
+      <c r="A193" s="4"/>
       <c r="B193" s="2" t="s">
         <v>31</v>
       </c>
-      <c r="C193" s="4"/>
+      <c r="C193" s="3"/>
     </row>
     <row r="194" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A194" s="5">
+      <c r="A194" s="4">
         <v>97</v>
       </c>
       <c r="B194" s="1" t="s">
         <v>245</v>
       </c>
-      <c r="C194" s="4" t="s">
+      <c r="C194" s="3" t="s">
         <v>247</v>
       </c>
     </row>
     <row r="195" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A195" s="5"/>
+      <c r="A195" s="4"/>
       <c r="B195" s="2" t="s">
         <v>246</v>
       </c>
-      <c r="C195" s="4"/>
+      <c r="C195" s="3"/>
     </row>
     <row r="196" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A196" s="5">
+      <c r="A196" s="4">
         <v>98</v>
       </c>
       <c r="B196" s="1" t="s">
         <v>248</v>
       </c>
-      <c r="C196" s="4" t="s">
+      <c r="C196" s="3" t="s">
         <v>250</v>
       </c>
     </row>
     <row r="197" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A197" s="5"/>
+      <c r="A197" s="4"/>
       <c r="B197" s="2" t="s">
         <v>249</v>
       </c>
-      <c r="C197" s="4"/>
+      <c r="C197" s="3"/>
     </row>
     <row r="198" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A198" s="5">
+      <c r="A198" s="4">
         <v>99</v>
       </c>
       <c r="B198" s="1" t="s">
         <v>251</v>
       </c>
-      <c r="C198" s="4" t="s">
+      <c r="C198" s="3" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="199" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A199" s="5"/>
+      <c r="A199" s="4"/>
       <c r="B199" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C199" s="4"/>
+      <c r="C199" s="3"/>
     </row>
     <row r="200" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A200" s="5">
+      <c r="A200" s="4">
         <v>100</v>
       </c>
       <c r="B200" s="1" t="s">
         <v>253</v>
       </c>
-      <c r="C200" s="4" t="s">
+      <c r="C200" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="201" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A201" s="5"/>
+      <c r="A201" s="4"/>
       <c r="B201" s="2" t="s">
         <v>149</v>
       </c>
-      <c r="C201" s="4"/>
+      <c r="C201" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="198">
-    <mergeCell ref="C4:C5"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="A2:A3"/>
-    <mergeCell ref="C10:C11"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="C8:C9"/>
-    <mergeCell ref="A8:A9"/>
-    <mergeCell ref="C6:C7"/>
-    <mergeCell ref="A6:A7"/>
-    <mergeCell ref="C16:C17"/>
-    <mergeCell ref="A16:A17"/>
-    <mergeCell ref="C14:C15"/>
-    <mergeCell ref="A14:A15"/>
-    <mergeCell ref="C12:C13"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="C22:C23"/>
-    <mergeCell ref="A22:A23"/>
-    <mergeCell ref="C20:C21"/>
-    <mergeCell ref="A20:A21"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="C30:C31"/>
-    <mergeCell ref="A30:A31"/>
-    <mergeCell ref="C28:C29"/>
-    <mergeCell ref="A28:A29"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="C24:C25"/>
-    <mergeCell ref="A24:A25"/>
-    <mergeCell ref="C36:C37"/>
-    <mergeCell ref="A36:A37"/>
-    <mergeCell ref="C34:C35"/>
-    <mergeCell ref="A34:A35"/>
-    <mergeCell ref="C32:C33"/>
-    <mergeCell ref="A32:A33"/>
-    <mergeCell ref="C42:C43"/>
-    <mergeCell ref="A42:A43"/>
-    <mergeCell ref="C40:C41"/>
-    <mergeCell ref="A40:A41"/>
-    <mergeCell ref="C38:C39"/>
-    <mergeCell ref="A38:A39"/>
-    <mergeCell ref="C48:C49"/>
-    <mergeCell ref="A48:A49"/>
-    <mergeCell ref="C46:C47"/>
-    <mergeCell ref="A46:A47"/>
-    <mergeCell ref="C44:C45"/>
-    <mergeCell ref="A44:A45"/>
-    <mergeCell ref="C54:C55"/>
-    <mergeCell ref="A54:A55"/>
-    <mergeCell ref="C52:C53"/>
-    <mergeCell ref="A52:A53"/>
-    <mergeCell ref="C50:C51"/>
-    <mergeCell ref="A50:A51"/>
-    <mergeCell ref="C60:C61"/>
-    <mergeCell ref="A60:A61"/>
-    <mergeCell ref="C58:C59"/>
-    <mergeCell ref="A58:A59"/>
-    <mergeCell ref="C56:C57"/>
-    <mergeCell ref="A56:A57"/>
-    <mergeCell ref="C66:C67"/>
-    <mergeCell ref="A66:A67"/>
-    <mergeCell ref="C64:C65"/>
-    <mergeCell ref="A64:A65"/>
-    <mergeCell ref="C62:C63"/>
-    <mergeCell ref="A62:A63"/>
-    <mergeCell ref="C72:C73"/>
-    <mergeCell ref="A72:A73"/>
-    <mergeCell ref="C70:C71"/>
-    <mergeCell ref="A70:A71"/>
-    <mergeCell ref="C68:C69"/>
-    <mergeCell ref="A68:A69"/>
-    <mergeCell ref="C80:C81"/>
-    <mergeCell ref="A80:A81"/>
-    <mergeCell ref="A78:A79"/>
-    <mergeCell ref="C76:C77"/>
-    <mergeCell ref="A76:A77"/>
-    <mergeCell ref="C74:C75"/>
-    <mergeCell ref="A74:A75"/>
-    <mergeCell ref="C86:C87"/>
-    <mergeCell ref="A86:A87"/>
-    <mergeCell ref="C84:C85"/>
-    <mergeCell ref="A84:A85"/>
-    <mergeCell ref="C82:C83"/>
-    <mergeCell ref="A82:A83"/>
-    <mergeCell ref="C92:C93"/>
-    <mergeCell ref="A92:A93"/>
-    <mergeCell ref="C90:C91"/>
-    <mergeCell ref="A90:A91"/>
-    <mergeCell ref="C88:C89"/>
-    <mergeCell ref="A88:A89"/>
-    <mergeCell ref="C98:C99"/>
-    <mergeCell ref="A98:A99"/>
-    <mergeCell ref="C96:C97"/>
-    <mergeCell ref="A96:A97"/>
-    <mergeCell ref="C94:C95"/>
-    <mergeCell ref="A94:A95"/>
-    <mergeCell ref="C104:C105"/>
-    <mergeCell ref="A104:A105"/>
-    <mergeCell ref="C102:C103"/>
-    <mergeCell ref="A102:A103"/>
-    <mergeCell ref="C100:C101"/>
-    <mergeCell ref="A100:A101"/>
-    <mergeCell ref="C110:C111"/>
-    <mergeCell ref="A110:A111"/>
-    <mergeCell ref="C108:C109"/>
-    <mergeCell ref="A108:A109"/>
-    <mergeCell ref="C106:C107"/>
-    <mergeCell ref="A106:A107"/>
-    <mergeCell ref="C116:C117"/>
-    <mergeCell ref="A116:A117"/>
-    <mergeCell ref="C114:C115"/>
-    <mergeCell ref="A114:A115"/>
-    <mergeCell ref="C112:C113"/>
-    <mergeCell ref="A112:A113"/>
-    <mergeCell ref="C122:C123"/>
-    <mergeCell ref="A122:A123"/>
-    <mergeCell ref="C120:C121"/>
-    <mergeCell ref="A120:A121"/>
-    <mergeCell ref="C118:C119"/>
-    <mergeCell ref="A118:A119"/>
-    <mergeCell ref="C128:C129"/>
-    <mergeCell ref="A128:A129"/>
-    <mergeCell ref="C126:C127"/>
-    <mergeCell ref="A126:A127"/>
-    <mergeCell ref="C124:C125"/>
-    <mergeCell ref="A124:A125"/>
-    <mergeCell ref="C134:C135"/>
-    <mergeCell ref="A134:A135"/>
-    <mergeCell ref="C132:C133"/>
-    <mergeCell ref="A132:A133"/>
-    <mergeCell ref="C130:C131"/>
-    <mergeCell ref="A130:A131"/>
-    <mergeCell ref="C140:C141"/>
-    <mergeCell ref="A140:A141"/>
-    <mergeCell ref="C138:C139"/>
-    <mergeCell ref="A138:A139"/>
-    <mergeCell ref="C136:C137"/>
-    <mergeCell ref="A136:A137"/>
-    <mergeCell ref="C146:C147"/>
-    <mergeCell ref="A146:A147"/>
-    <mergeCell ref="C144:C145"/>
-    <mergeCell ref="A144:A145"/>
-    <mergeCell ref="C142:C143"/>
-    <mergeCell ref="A142:A143"/>
-    <mergeCell ref="C152:C153"/>
-    <mergeCell ref="A152:A153"/>
-    <mergeCell ref="C150:C151"/>
-    <mergeCell ref="A150:A151"/>
-    <mergeCell ref="C148:C149"/>
-    <mergeCell ref="A148:A149"/>
-    <mergeCell ref="C158:C159"/>
-    <mergeCell ref="A158:A159"/>
-    <mergeCell ref="C156:C157"/>
-    <mergeCell ref="A156:A157"/>
-    <mergeCell ref="C154:C155"/>
-    <mergeCell ref="A154:A155"/>
-    <mergeCell ref="C164:C165"/>
-    <mergeCell ref="A164:A165"/>
-    <mergeCell ref="C162:C163"/>
-    <mergeCell ref="A162:A163"/>
-    <mergeCell ref="C160:C161"/>
-    <mergeCell ref="A160:A161"/>
-    <mergeCell ref="C170:C171"/>
-    <mergeCell ref="A170:A171"/>
-    <mergeCell ref="C168:C169"/>
-    <mergeCell ref="A168:A169"/>
-    <mergeCell ref="C166:C167"/>
-    <mergeCell ref="A166:A167"/>
-    <mergeCell ref="C176:C177"/>
-    <mergeCell ref="A176:A177"/>
-    <mergeCell ref="C174:C175"/>
-    <mergeCell ref="A174:A175"/>
-    <mergeCell ref="C172:C173"/>
-    <mergeCell ref="A172:A173"/>
-    <mergeCell ref="C182:C183"/>
-    <mergeCell ref="A182:A183"/>
-    <mergeCell ref="C180:C181"/>
-    <mergeCell ref="A180:A181"/>
-    <mergeCell ref="C178:C179"/>
-    <mergeCell ref="A178:A179"/>
-    <mergeCell ref="C188:C189"/>
-    <mergeCell ref="A188:A189"/>
-    <mergeCell ref="C186:C187"/>
-    <mergeCell ref="A186:A187"/>
-    <mergeCell ref="C184:C185"/>
-    <mergeCell ref="A184:A185"/>
-    <mergeCell ref="C194:C195"/>
-    <mergeCell ref="A194:A195"/>
-    <mergeCell ref="C192:C193"/>
-    <mergeCell ref="A192:A193"/>
-    <mergeCell ref="C190:C191"/>
-    <mergeCell ref="A190:A191"/>
-    <mergeCell ref="C200:C201"/>
-    <mergeCell ref="A200:A201"/>
-    <mergeCell ref="C198:C199"/>
-    <mergeCell ref="A198:A199"/>
-    <mergeCell ref="C196:C197"/>
-    <mergeCell ref="A196:A197"/>
-  </mergeCells>
   <hyperlinks>
     <hyperlink ref="B2" r:id="rId1"/>
     <hyperlink ref="B4" r:id="rId2"/>

</xml_diff>